<commit_message>
input and output files removed
</commit_message>
<xml_diff>
--- a/scripts/us_epa/air_emissions_inventory/national_state/test_files/input_files/state_tier1_ktons.xlsx
+++ b/scripts/us_epa/air_emissions_inventory/national_state/test_files/input_files/state_tier1_ktons.xlsx
@@ -13,7 +13,7 @@
     <sheet name="State_Trends" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">State_Trends!$A$2:$AH$20</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">State_Trends!$A$2:$AH$8</definedName>
     <definedName function="false" hidden="false" name="_SAS_empty_" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="151">
   <si>
     <t xml:space="preserve">All Emissions in this workbook are in kilotons (1000 short tons=2,000,000 lbs)</t>
   </si>
@@ -566,25 +566,22 @@
     <t xml:space="preserve">CO</t>
   </si>
   <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical &amp; Allied Product Mfg</t>
+  </si>
+  <si>
     <t xml:space="preserve">NH3</t>
   </si>
   <si>
-    <t xml:space="preserve">PM10-PRI</t>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wildfires</t>
   </si>
   <si>
     <t xml:space="preserve">VOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical &amp; Allied Product Mfg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wildfires</t>
   </si>
   <si>
     <t xml:space="preserve">02</t>
@@ -1692,14 +1689,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH1048576"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="Z123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
-      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
-      <selection pane="bottomRight" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1933,97 +1930,100 @@
         <v>140</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>54.70092</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.01516</v>
+        <v>44.2331</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0.01605</v>
+        <v>45.59779</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.01597</v>
+        <v>46.96713</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.01651</v>
+        <v>7.85382</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.016949</v>
+        <v>8.090869</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.015926</v>
+        <v>8.309889</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.788501899</v>
+        <v>5.7214050302</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>0.788501899</v>
+        <v>5.7214050302</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>0.624737763</v>
+        <v>7.2078657362</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>0.624737763</v>
+        <v>7.2078657362</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>0.6193367197</v>
+        <v>1.040698102</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.5904185747</v>
+        <v>1.040698102</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0.5904185747</v>
+        <v>1.040698102</v>
       </c>
       <c r="T4" s="1" t="n">
-        <v>0.4174618898</v>
+        <v>2.225352501</v>
       </c>
       <c r="U4" s="1" t="n">
-        <v>0.43155819</v>
+        <v>3.122954911</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>0.48931921</v>
+        <v>3.122954911</v>
       </c>
       <c r="W4" s="1" t="n">
-        <v>0.542951832</v>
+        <v>3.122954911</v>
       </c>
       <c r="X4" s="1" t="n">
-        <v>0.55705216</v>
+        <v>2.951498996</v>
       </c>
       <c r="Y4" s="1" t="n">
-        <v>0.48674935</v>
+        <v>3.1350329643</v>
       </c>
       <c r="Z4" s="1" t="n">
-        <v>0.328625</v>
+        <v>3.258271986</v>
       </c>
       <c r="AA4" s="1" t="n">
-        <v>0.31078297</v>
+        <v>3.0543673395</v>
       </c>
       <c r="AB4" s="1" t="n">
-        <v>0.3988731204</v>
+        <v>3.3311576904</v>
       </c>
       <c r="AC4" s="1" t="n">
-        <v>0.45576019</v>
+        <v>2.700596875</v>
       </c>
       <c r="AD4" s="1" t="n">
-        <v>0.4175513321</v>
+        <v>2.626483677</v>
       </c>
       <c r="AE4" s="1" t="n">
-        <v>0.551173926</v>
+        <v>2.6349189402</v>
       </c>
       <c r="AF4" s="1" t="n">
-        <v>0.640021549</v>
+        <v>2.659693238</v>
       </c>
       <c r="AG4" s="1" t="n">
-        <v>0.717073903</v>
+        <v>1.9393069255</v>
       </c>
       <c r="AH4" s="1" t="n">
-        <v>0.717073903</v>
+        <v>1.9393069255</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,100 +2034,100 @@
         <v>140</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>8.85994</v>
+        <v>3.21457</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>9.28102</v>
+        <v>2.29521</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>8.83472</v>
+        <v>2.35559</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>8.37946</v>
+        <v>2.48176</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>29.21702</v>
+        <v>0.01122</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>28.920119</v>
+        <v>0.011589</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>27.213014</v>
+        <v>0.011886</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>26.03978518</v>
+        <v>0.0348299999</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>26.03978518</v>
+        <v>0.0348299999</v>
       </c>
       <c r="O5" s="1" t="n">
-        <v>27.007889443</v>
+        <v>0.0347254286</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>27.007889443</v>
+        <v>0.0347254286</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>26.832423959</v>
+        <v>0.030830001</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>5.7429826949</v>
+        <v>0.030830001</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>5.7429826949</v>
+        <v>0.030830001</v>
       </c>
       <c r="T5" s="1" t="n">
-        <v>3.3099615669</v>
+        <v>0.0340177</v>
       </c>
       <c r="U5" s="1" t="n">
-        <v>3.3491298491</v>
+        <v>0.182615</v>
       </c>
       <c r="V5" s="1" t="n">
-        <v>7.3233217787</v>
+        <v>0.182615</v>
       </c>
       <c r="W5" s="1" t="n">
-        <v>4.7412628553</v>
+        <v>0.182615</v>
       </c>
       <c r="X5" s="1" t="n">
-        <v>5.7463797784</v>
+        <v>0.1349816501</v>
       </c>
       <c r="Y5" s="1" t="n">
-        <v>4.7633005492</v>
+        <v>0.1271626169</v>
       </c>
       <c r="Z5" s="1" t="n">
-        <v>4.3647039969</v>
+        <v>0.109666436</v>
       </c>
       <c r="AA5" s="1" t="n">
-        <v>2.1047387932</v>
+        <v>0.1467694153</v>
       </c>
       <c r="AB5" s="1" t="n">
-        <v>2.3260056864</v>
+        <v>0.159389196</v>
       </c>
       <c r="AC5" s="1" t="n">
-        <v>2.6010103892</v>
+        <v>0.145965147</v>
       </c>
       <c r="AD5" s="1" t="n">
-        <v>2.8686421139</v>
+        <v>0.085213461</v>
       </c>
       <c r="AE5" s="1" t="n">
-        <v>1.5941560078</v>
+        <v>0.097356034</v>
       </c>
       <c r="AF5" s="1" t="n">
-        <v>1.7405704304</v>
+        <v>0.098254668</v>
       </c>
       <c r="AG5" s="1" t="n">
-        <v>1.7597839679</v>
+        <v>0.256630415</v>
       </c>
       <c r="AH5" s="1" t="n">
-        <v>1.7597839679</v>
+        <v>0.256630415</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,100 +2138,79 @@
         <v>140</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.79719</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0.99511</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>0.9925</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>1.00374</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>2.23487</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>2.133452</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>2.105723</v>
+        <v>142</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>2.259568003</v>
+        <v>28.793369</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>2.259568003</v>
+        <v>0</v>
       </c>
       <c r="O6" s="1" t="n">
-        <v>1.90810461</v>
+        <v>8.344</v>
       </c>
       <c r="P6" s="1" t="n">
-        <v>1.90810461</v>
+        <v>26.042884</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>1.90976234</v>
+        <v>28.1842226</v>
       </c>
       <c r="R6" s="1" t="n">
-        <v>1.6800374059</v>
+        <v>38.128038</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>1.6800374059</v>
+        <v>7.7495436</v>
       </c>
       <c r="T6" s="1" t="n">
-        <v>1.2617460032</v>
+        <v>4.2539279</v>
       </c>
       <c r="U6" s="1" t="n">
-        <v>1.0896396597</v>
+        <v>12.0268997</v>
       </c>
       <c r="V6" s="1" t="n">
-        <v>1.1517990537</v>
+        <v>36.5804084</v>
       </c>
       <c r="W6" s="1" t="n">
-        <v>1.3075699398</v>
+        <v>9.1453743</v>
       </c>
       <c r="X6" s="1" t="n">
-        <v>1.477690241</v>
+        <v>13.3745838</v>
       </c>
       <c r="Y6" s="1" t="n">
-        <v>1.3480152001</v>
+        <v>12.9995432</v>
       </c>
       <c r="Z6" s="1" t="n">
-        <v>1.2238769203</v>
+        <v>12.2603596</v>
       </c>
       <c r="AA6" s="1" t="n">
-        <v>1.1932657881</v>
+        <v>82.049138</v>
       </c>
       <c r="AB6" s="1" t="n">
-        <v>1.2130126517</v>
+        <v>2.18414666</v>
       </c>
       <c r="AC6" s="1" t="n">
-        <v>1.316165274</v>
+        <v>23.527953</v>
       </c>
       <c r="AD6" s="1" t="n">
-        <v>1.1835841508</v>
+        <v>38.780561</v>
       </c>
       <c r="AE6" s="1" t="n">
-        <v>1.01798711</v>
+        <v>3.049515266</v>
       </c>
       <c r="AF6" s="1" t="n">
-        <v>1.089432182</v>
+        <v>4.985326435</v>
       </c>
       <c r="AG6" s="1" t="n">
-        <v>1.128973959</v>
+        <v>21.425489124</v>
       </c>
       <c r="AH6" s="1" t="n">
-        <v>1.128973959</v>
+        <v>21.425489124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2248,1900 +2227,181 @@
         <v>147</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>54.70092</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>44.2331</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>45.59779</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>46.96713</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>7.85382</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>8.090869</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>8.309889</v>
+        <v>148</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>5.7214050302</v>
+        <v>6.846048</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>5.7214050302</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1" t="n">
-        <v>7.2078657362</v>
+        <v>1.98419812</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>7.2078657362</v>
+        <v>6.18674437</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>1.040698102</v>
+        <v>6.6974117</v>
       </c>
       <c r="R7" s="1" t="n">
-        <v>1.040698102</v>
+        <v>9.0612204</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>1.040698102</v>
+        <v>1.84221012</v>
       </c>
       <c r="T7" s="1" t="n">
-        <v>2.225352501</v>
+        <v>1.01145249</v>
       </c>
       <c r="U7" s="1" t="n">
-        <v>3.122954911</v>
+        <v>2.85839828</v>
       </c>
       <c r="V7" s="1" t="n">
-        <v>3.122954911</v>
+        <v>8.6908201</v>
       </c>
       <c r="W7" s="1" t="n">
-        <v>3.122954911</v>
+        <v>2.16964072</v>
       </c>
       <c r="X7" s="1" t="n">
-        <v>2.951498996</v>
+        <v>3.1770981</v>
       </c>
       <c r="Y7" s="1" t="n">
-        <v>3.1350329643</v>
+        <v>3.08977135</v>
       </c>
       <c r="Z7" s="1" t="n">
-        <v>3.258271986</v>
+        <v>2.91535496</v>
       </c>
       <c r="AA7" s="1" t="n">
-        <v>3.0543673395</v>
+        <v>19.5219497</v>
       </c>
       <c r="AB7" s="1" t="n">
-        <v>3.3311576904</v>
+        <v>0.51894634</v>
       </c>
       <c r="AC7" s="1" t="n">
-        <v>2.700596875</v>
+        <v>5.58987654</v>
       </c>
       <c r="AD7" s="1" t="n">
-        <v>2.626483677</v>
+        <v>9.229566</v>
       </c>
       <c r="AE7" s="1" t="n">
-        <v>2.6349189402</v>
+        <v>0.7258877677</v>
       </c>
       <c r="AF7" s="1" t="n">
-        <v>2.659693238</v>
+        <v>1.592170435</v>
       </c>
       <c r="AG7" s="1" t="n">
-        <v>1.9393069255</v>
+        <v>7.185328706</v>
       </c>
       <c r="AH7" s="1" t="n">
-        <v>1.9393069255</v>
+        <v>7.185328706</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>146</v>
-      </c>
       <c r="D8" s="14" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>3.21457</v>
+        <v>0.59919</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>2.29521</v>
+        <v>2.75036</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>2.35559</v>
+        <v>2.81292</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>2.48176</v>
+        <v>2.87542</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>0.01122</v>
+        <v>2.95033</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>0.011589</v>
+        <v>3.030148</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>0.011886</v>
+        <v>3.098005</v>
       </c>
       <c r="M8" s="1" t="n">
-        <v>0.0348299999</v>
+        <v>6.61341002</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>0.0348299999</v>
+        <v>6.61341002</v>
       </c>
       <c r="O8" s="1" t="n">
-        <v>0.0347254286</v>
+        <v>7.190790005</v>
       </c>
       <c r="P8" s="1" t="n">
-        <v>0.0347254286</v>
+        <v>7.190790005</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>0.030830001</v>
+        <v>6.005299999</v>
       </c>
       <c r="R8" s="1" t="n">
-        <v>0.030830001</v>
+        <v>6.005299999</v>
       </c>
       <c r="S8" s="1" t="n">
-        <v>0.030830001</v>
+        <v>6.005299999</v>
       </c>
       <c r="T8" s="1" t="n">
-        <v>0.0340177</v>
+        <v>5.8207300001</v>
       </c>
       <c r="U8" s="1" t="n">
-        <v>0.182615</v>
+        <v>4.814950001</v>
       </c>
       <c r="V8" s="1" t="n">
-        <v>0.182615</v>
+        <v>4.814950001</v>
       </c>
       <c r="W8" s="1" t="n">
-        <v>0.182615</v>
+        <v>4.814950001</v>
       </c>
       <c r="X8" s="1" t="n">
-        <v>0.1349816501</v>
+        <v>4.121540001</v>
       </c>
       <c r="Y8" s="1" t="n">
-        <v>0.1271626169</v>
+        <v>4.74111</v>
       </c>
       <c r="Z8" s="1" t="n">
-        <v>0.109666436</v>
+        <v>4.869100001</v>
       </c>
       <c r="AA8" s="1" t="n">
-        <v>0.1467694153</v>
+        <v>3.824213244</v>
       </c>
       <c r="AB8" s="1" t="n">
-        <v>0.159389196</v>
+        <v>4.4833331999</v>
       </c>
       <c r="AC8" s="1" t="n">
-        <v>0.145965147</v>
+        <v>5.134883169</v>
       </c>
       <c r="AD8" s="1" t="n">
-        <v>0.085213461</v>
+        <v>4.678804456</v>
       </c>
       <c r="AE8" s="1" t="n">
-        <v>0.097356034</v>
+        <v>4.7466041</v>
       </c>
       <c r="AF8" s="1" t="n">
-        <v>0.098254668</v>
+        <v>4.6391257</v>
       </c>
       <c r="AG8" s="1" t="n">
-        <v>0.256630415</v>
+        <v>4.6384374</v>
       </c>
       <c r="AH8" s="1" t="n">
-        <v>0.256630415</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>1.01733</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>1.0479</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>1.0728</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>1.10829</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>1.068639</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>1.09872</v>
-      </c>
-      <c r="L9" s="1" t="n">
-        <v>1.127882</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>1.1544617808</v>
-      </c>
-      <c r="N9" s="1" t="n">
-        <v>1.1544617808</v>
-      </c>
-      <c r="O9" s="1" t="n">
-        <v>1.0206744506</v>
-      </c>
-      <c r="P9" s="1" t="n">
-        <v>1.0206744506</v>
-      </c>
-      <c r="Q9" s="1" t="n">
-        <v>0.6432348066</v>
-      </c>
-      <c r="R9" s="1" t="n">
-        <v>0.6432348066</v>
-      </c>
-      <c r="S9" s="1" t="n">
-        <v>0.6432348066</v>
-      </c>
-      <c r="T9" s="1" t="n">
-        <v>0.5396427496</v>
-      </c>
-      <c r="U9" s="1" t="n">
-        <v>0.7041153736</v>
-      </c>
-      <c r="V9" s="1" t="n">
-        <v>0.7041153736</v>
-      </c>
-      <c r="W9" s="1" t="n">
-        <v>0.7041153736</v>
-      </c>
-      <c r="X9" s="1" t="n">
-        <v>0.7118373592</v>
-      </c>
-      <c r="Y9" s="1" t="n">
-        <v>0.7055228141</v>
-      </c>
-      <c r="Z9" s="1" t="n">
-        <v>0.6930940453</v>
-      </c>
-      <c r="AA9" s="1" t="n">
-        <v>0.7003185247</v>
-      </c>
-      <c r="AB9" s="1" t="n">
-        <v>0.6813309664</v>
-      </c>
-      <c r="AC9" s="1" t="n">
-        <v>0.6972949382</v>
-      </c>
-      <c r="AD9" s="1" t="n">
-        <v>0.5676728648</v>
-      </c>
-      <c r="AE9" s="1" t="n">
-        <v>0.9425716698</v>
-      </c>
-      <c r="AF9" s="1" t="n">
-        <v>0.9018041343</v>
-      </c>
-      <c r="AG9" s="1" t="n">
-        <v>0.7750260365</v>
-      </c>
-      <c r="AH9" s="1" t="n">
-        <v>0.7750260365</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>23.18752</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>32.10071</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>33.00012</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>33.97481</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <v>15.82141</v>
-      </c>
-      <c r="K10" s="1" t="n">
-        <v>16.296737</v>
-      </c>
-      <c r="L10" s="1" t="n">
-        <v>16.796007</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>9.839787799</v>
-      </c>
-      <c r="N10" s="1" t="n">
-        <v>9.839787799</v>
-      </c>
-      <c r="O10" s="1" t="n">
-        <v>8.9289371066</v>
-      </c>
-      <c r="P10" s="1" t="n">
-        <v>8.9289371066</v>
-      </c>
-      <c r="Q10" s="1" t="n">
-        <v>1.4590704013</v>
-      </c>
-      <c r="R10" s="1" t="n">
-        <v>1.4566824013</v>
-      </c>
-      <c r="S10" s="1" t="n">
-        <v>1.4566824013</v>
-      </c>
-      <c r="T10" s="1" t="n">
-        <v>1.2873506446</v>
-      </c>
-      <c r="U10" s="1" t="n">
-        <v>1.629337687</v>
-      </c>
-      <c r="V10" s="1" t="n">
-        <v>1.629337687</v>
-      </c>
-      <c r="W10" s="1" t="n">
-        <v>1.629337687</v>
-      </c>
-      <c r="X10" s="1" t="n">
-        <v>1.54309364</v>
-      </c>
-      <c r="Y10" s="1" t="n">
-        <v>1.5760694139</v>
-      </c>
-      <c r="Z10" s="1" t="n">
-        <v>1.6486328256</v>
-      </c>
-      <c r="AA10" s="1" t="n">
-        <v>1.559075957</v>
-      </c>
-      <c r="AB10" s="1" t="n">
-        <v>1.6794087346</v>
-      </c>
-      <c r="AC10" s="1" t="n">
-        <v>1.5180669249</v>
-      </c>
-      <c r="AD10" s="1" t="n">
-        <v>1.4533002129</v>
-      </c>
-      <c r="AE10" s="1" t="n">
-        <v>1.3796840495</v>
-      </c>
-      <c r="AF10" s="1" t="n">
-        <v>1.3607663786</v>
-      </c>
-      <c r="AG10" s="1" t="n">
-        <v>1.3322474502</v>
-      </c>
-      <c r="AH10" s="1" t="n">
-        <v>1.3322474502</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="M11" s="1" t="n">
-        <v>28.793369</v>
-      </c>
-      <c r="N11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1" t="n">
-        <v>8.344</v>
-      </c>
-      <c r="P11" s="1" t="n">
-        <v>26.042884</v>
-      </c>
-      <c r="Q11" s="1" t="n">
-        <v>28.1842226</v>
-      </c>
-      <c r="R11" s="1" t="n">
-        <v>38.128038</v>
-      </c>
-      <c r="S11" s="1" t="n">
-        <v>7.7495436</v>
-      </c>
-      <c r="T11" s="1" t="n">
-        <v>4.2539279</v>
-      </c>
-      <c r="U11" s="1" t="n">
-        <v>12.0268997</v>
-      </c>
-      <c r="V11" s="1" t="n">
-        <v>36.5804084</v>
-      </c>
-      <c r="W11" s="1" t="n">
-        <v>9.1453743</v>
-      </c>
-      <c r="X11" s="1" t="n">
-        <v>13.3745838</v>
-      </c>
-      <c r="Y11" s="1" t="n">
-        <v>12.9995432</v>
-      </c>
-      <c r="Z11" s="1" t="n">
-        <v>12.2603596</v>
-      </c>
-      <c r="AA11" s="1" t="n">
-        <v>82.049138</v>
-      </c>
-      <c r="AB11" s="1" t="n">
-        <v>2.18414666</v>
-      </c>
-      <c r="AC11" s="1" t="n">
-        <v>23.527953</v>
-      </c>
-      <c r="AD11" s="1" t="n">
-        <v>38.780561</v>
-      </c>
-      <c r="AE11" s="1" t="n">
-        <v>3.049515266</v>
-      </c>
-      <c r="AF11" s="1" t="n">
-        <v>4.985326435</v>
-      </c>
-      <c r="AG11" s="1" t="n">
-        <v>21.425489124</v>
-      </c>
-      <c r="AH11" s="1" t="n">
-        <v>21.425489124</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="M12" s="1" t="n">
-        <v>0.4762468</v>
-      </c>
-      <c r="N12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1" t="n">
-        <v>0.138031171</v>
-      </c>
-      <c r="P12" s="1" t="n">
-        <v>0.43038221</v>
-      </c>
-      <c r="Q12" s="1" t="n">
-        <v>0.46590693</v>
-      </c>
-      <c r="R12" s="1" t="n">
-        <v>0.63034572</v>
-      </c>
-      <c r="S12" s="1" t="n">
-        <v>0.128153752</v>
-      </c>
-      <c r="T12" s="1" t="n">
-        <v>0.070361922</v>
-      </c>
-      <c r="U12" s="1" t="n">
-        <v>0.198845095</v>
-      </c>
-      <c r="V12" s="1" t="n">
-        <v>0.60457881</v>
-      </c>
-      <c r="W12" s="1" t="n">
-        <v>0.150931537</v>
-      </c>
-      <c r="X12" s="1" t="n">
-        <v>0.221015506</v>
-      </c>
-      <c r="Y12" s="1" t="n">
-        <v>0.214940615</v>
-      </c>
-      <c r="Z12" s="1" t="n">
-        <v>0.20280731</v>
-      </c>
-      <c r="AA12" s="1" t="n">
-        <v>1.35804737</v>
-      </c>
-      <c r="AB12" s="1" t="n">
-        <v>0.036100608</v>
-      </c>
-      <c r="AC12" s="1" t="n">
-        <v>0.388860996</v>
-      </c>
-      <c r="AD12" s="1" t="n">
-        <v>0.64205676</v>
-      </c>
-      <c r="AE12" s="1" t="n">
-        <v>0.0504965421</v>
-      </c>
-      <c r="AF12" s="1" t="n">
-        <v>0.077757753</v>
-      </c>
-      <c r="AG12" s="1" t="n">
-        <v>0.250331755</v>
-      </c>
-      <c r="AH12" s="1" t="n">
-        <v>0.250331755</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="M13" s="1" t="n">
-        <v>3.09800093</v>
-      </c>
-      <c r="N13" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1" t="n">
-        <v>0.898690586</v>
-      </c>
-      <c r="P13" s="1" t="n">
-        <v>2.78500068</v>
-      </c>
-      <c r="Q13" s="1" t="n">
-        <v>3.0202975</v>
-      </c>
-      <c r="R13" s="1" t="n">
-        <v>4.08865787</v>
-      </c>
-      <c r="S13" s="1" t="n">
-        <v>0.83266031</v>
-      </c>
-      <c r="T13" s="1" t="n">
-        <v>0.457756955</v>
-      </c>
-      <c r="U13" s="1" t="n">
-        <v>1.29026886</v>
-      </c>
-      <c r="V13" s="1" t="n">
-        <v>3.9143751</v>
-      </c>
-      <c r="W13" s="1" t="n">
-        <v>0.96861538</v>
-      </c>
-      <c r="X13" s="1" t="n">
-        <v>1.42973193</v>
-      </c>
-      <c r="Y13" s="1" t="n">
-        <v>1.39528005</v>
-      </c>
-      <c r="Z13" s="1" t="n">
-        <v>1.32002</v>
-      </c>
-      <c r="AA13" s="1" t="n">
-        <v>8.8713807</v>
-      </c>
-      <c r="AB13" s="1" t="n">
-        <v>0.233828641</v>
-      </c>
-      <c r="AC13" s="1" t="n">
-        <v>2.51790616</v>
-      </c>
-      <c r="AD13" s="1" t="n">
-        <v>4.20108024</v>
-      </c>
-      <c r="AE13" s="1" t="n">
-        <v>0.3307342416</v>
-      </c>
-      <c r="AF13" s="1" t="n">
-        <v>1.129058716</v>
-      </c>
-      <c r="AG13" s="1" t="n">
-        <v>5.436198881</v>
-      </c>
-      <c r="AH13" s="1" t="n">
-        <v>5.436198881</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="M14" s="1" t="n">
-        <v>6.846048</v>
-      </c>
-      <c r="N14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1" t="n">
-        <v>1.98419812</v>
-      </c>
-      <c r="P14" s="1" t="n">
-        <v>6.18674437</v>
-      </c>
-      <c r="Q14" s="1" t="n">
-        <v>6.6974117</v>
-      </c>
-      <c r="R14" s="1" t="n">
-        <v>9.0612204</v>
-      </c>
-      <c r="S14" s="1" t="n">
-        <v>1.84221012</v>
-      </c>
-      <c r="T14" s="1" t="n">
-        <v>1.01145249</v>
-      </c>
-      <c r="U14" s="1" t="n">
-        <v>2.85839828</v>
-      </c>
-      <c r="V14" s="1" t="n">
-        <v>8.6908201</v>
-      </c>
-      <c r="W14" s="1" t="n">
-        <v>2.16964072</v>
-      </c>
-      <c r="X14" s="1" t="n">
-        <v>3.1770981</v>
-      </c>
-      <c r="Y14" s="1" t="n">
-        <v>3.08977135</v>
-      </c>
-      <c r="Z14" s="1" t="n">
-        <v>2.91535496</v>
-      </c>
-      <c r="AA14" s="1" t="n">
-        <v>19.5219497</v>
-      </c>
-      <c r="AB14" s="1" t="n">
-        <v>0.51894634</v>
-      </c>
-      <c r="AC14" s="1" t="n">
-        <v>5.58987654</v>
-      </c>
-      <c r="AD14" s="1" t="n">
-        <v>9.229566</v>
-      </c>
-      <c r="AE14" s="1" t="n">
-        <v>0.7258877677</v>
-      </c>
-      <c r="AF14" s="1" t="n">
-        <v>1.592170435</v>
-      </c>
-      <c r="AG14" s="1" t="n">
-        <v>7.185328706</v>
-      </c>
-      <c r="AH14" s="1" t="n">
-        <v>7.185328706</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>0.59919</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>2.75036</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>2.81292</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>2.87542</v>
-      </c>
-      <c r="J15" s="1" t="n">
-        <v>2.95033</v>
-      </c>
-      <c r="K15" s="1" t="n">
-        <v>3.030148</v>
-      </c>
-      <c r="L15" s="1" t="n">
-        <v>3.098005</v>
-      </c>
-      <c r="M15" s="1" t="n">
-        <v>6.61341002</v>
-      </c>
-      <c r="N15" s="1" t="n">
-        <v>6.61341002</v>
-      </c>
-      <c r="O15" s="1" t="n">
-        <v>7.190790005</v>
-      </c>
-      <c r="P15" s="1" t="n">
-        <v>7.190790005</v>
-      </c>
-      <c r="Q15" s="1" t="n">
-        <v>6.005299999</v>
-      </c>
-      <c r="R15" s="1" t="n">
-        <v>6.005299999</v>
-      </c>
-      <c r="S15" s="1" t="n">
-        <v>6.005299999</v>
-      </c>
-      <c r="T15" s="1" t="n">
-        <v>5.8207300001</v>
-      </c>
-      <c r="U15" s="1" t="n">
-        <v>4.814950001</v>
-      </c>
-      <c r="V15" s="1" t="n">
-        <v>4.814950001</v>
-      </c>
-      <c r="W15" s="1" t="n">
-        <v>4.814950001</v>
-      </c>
-      <c r="X15" s="1" t="n">
-        <v>4.121540001</v>
-      </c>
-      <c r="Y15" s="1" t="n">
-        <v>4.74111</v>
-      </c>
-      <c r="Z15" s="1" t="n">
-        <v>4.869100001</v>
-      </c>
-      <c r="AA15" s="1" t="n">
-        <v>3.824213244</v>
-      </c>
-      <c r="AB15" s="1" t="n">
-        <v>4.4833331999</v>
-      </c>
-      <c r="AC15" s="1" t="n">
-        <v>5.134883169</v>
-      </c>
-      <c r="AD15" s="1" t="n">
-        <v>4.678804456</v>
-      </c>
-      <c r="AE15" s="1" t="n">
-        <v>4.7466041</v>
-      </c>
-      <c r="AF15" s="1" t="n">
-        <v>4.6391257</v>
-      </c>
-      <c r="AG15" s="1" t="n">
         <v>4.6384374</v>
       </c>
-      <c r="AH15" s="1" t="n">
-        <v>4.6384374</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>0.00033</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <v>0.00034</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="J16" s="1" t="n">
-        <v>0.00015</v>
-      </c>
-      <c r="K16" s="1" t="n">
-        <v>0.000105</v>
-      </c>
-      <c r="L16" s="1" t="n">
-        <v>0.000112</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="P16" s="1" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="Q16" s="1" t="n">
-        <v>0.16964</v>
-      </c>
-      <c r="R16" s="1" t="n">
-        <v>0.16964</v>
-      </c>
-      <c r="S16" s="1" t="n">
-        <v>0.16964</v>
-      </c>
-      <c r="T16" s="1" t="n">
-        <v>0.16964</v>
-      </c>
-      <c r="U16" s="1" t="n">
-        <v>0.01386</v>
-      </c>
-      <c r="V16" s="1" t="n">
-        <v>0.01386</v>
-      </c>
-      <c r="W16" s="1" t="n">
-        <v>0.01386</v>
-      </c>
-      <c r="X16" s="1" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="Y16" s="1" t="n">
-        <v>0.02228</v>
-      </c>
-      <c r="Z16" s="1" t="n">
-        <v>0.0223900001</v>
-      </c>
-      <c r="AA16" s="1" t="n">
-        <v>0.0167352</v>
-      </c>
-      <c r="AB16" s="1" t="n">
-        <v>0.0335820003</v>
-      </c>
-      <c r="AC16" s="1" t="n">
-        <v>0.0723372002</v>
-      </c>
-      <c r="AD16" s="1" t="n">
-        <v>0.0739941999</v>
-      </c>
-      <c r="AE16" s="1" t="n">
-        <v>0.0528683</v>
-      </c>
-      <c r="AF16" s="1" t="n">
-        <v>0.0396364</v>
-      </c>
-      <c r="AG16" s="1" t="n">
-        <v>0.0381332</v>
-      </c>
-      <c r="AH16" s="1" t="n">
-        <v>0.0381332</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>0.41941</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>0.1815</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>0.1828</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>0.1886</v>
-      </c>
-      <c r="J17" s="1" t="n">
-        <v>0.218988</v>
-      </c>
-      <c r="K17" s="1" t="n">
-        <v>0.252235</v>
-      </c>
-      <c r="L17" s="1" t="n">
-        <v>0.251172</v>
-      </c>
-      <c r="M17" s="1" t="n">
-        <v>2.6171707593</v>
-      </c>
-      <c r="N17" s="1" t="n">
-        <v>2.6171707593</v>
-      </c>
-      <c r="O17" s="1" t="n">
-        <v>1.1326271</v>
-      </c>
-      <c r="P17" s="1" t="n">
-        <v>1.1326271</v>
-      </c>
-      <c r="Q17" s="1" t="n">
-        <v>0.6851400006</v>
-      </c>
-      <c r="R17" s="1" t="n">
-        <v>0.6851400006</v>
-      </c>
-      <c r="S17" s="1" t="n">
-        <v>0.6851400006</v>
-      </c>
-      <c r="T17" s="1" t="n">
-        <v>0.6847282</v>
-      </c>
-      <c r="U17" s="1" t="n">
-        <v>0.84629577</v>
-      </c>
-      <c r="V17" s="1" t="n">
-        <v>0.84629577</v>
-      </c>
-      <c r="W17" s="1" t="n">
-        <v>0.84629577</v>
-      </c>
-      <c r="X17" s="1" t="n">
-        <v>0.6928857699</v>
-      </c>
-      <c r="Y17" s="1" t="n">
-        <v>0.6175030805</v>
-      </c>
-      <c r="Z17" s="1" t="n">
-        <v>0.5279530769</v>
-      </c>
-      <c r="AA17" s="1" t="n">
-        <v>0.9222799351</v>
-      </c>
-      <c r="AB17" s="1" t="n">
-        <v>1.0082988732</v>
-      </c>
-      <c r="AC17" s="1" t="n">
-        <v>0.9588475005</v>
-      </c>
-      <c r="AD17" s="1" t="n">
-        <v>0.9676496319</v>
-      </c>
-      <c r="AE17" s="1" t="n">
-        <v>0.7663237843</v>
-      </c>
-      <c r="AF17" s="1" t="n">
-        <v>0.7544975843</v>
-      </c>
-      <c r="AG17" s="1" t="n">
-        <v>0.5045040843</v>
-      </c>
-      <c r="AH17" s="1" t="n">
-        <v>0.5045040843</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>0.3972</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>0.05989</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>0.06096</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>0.06201</v>
-      </c>
-      <c r="J18" s="1" t="n">
-        <v>0.06464</v>
-      </c>
-      <c r="K18" s="1" t="n">
-        <v>0.067869</v>
-      </c>
-      <c r="L18" s="1" t="n">
-        <v>0.070514</v>
-      </c>
-      <c r="M18" s="1" t="n">
-        <v>0.419890004</v>
-      </c>
-      <c r="N18" s="1" t="n">
-        <v>0.419890004</v>
-      </c>
-      <c r="O18" s="1" t="n">
-        <v>1.0549699991</v>
-      </c>
-      <c r="P18" s="1" t="n">
-        <v>1.0549699991</v>
-      </c>
-      <c r="Q18" s="1" t="n">
-        <v>0.8725300019</v>
-      </c>
-      <c r="R18" s="1" t="n">
-        <v>0.8725300019</v>
-      </c>
-      <c r="S18" s="1" t="n">
-        <v>0.8725300019</v>
-      </c>
-      <c r="T18" s="1" t="n">
-        <v>0.7563199999</v>
-      </c>
-      <c r="U18" s="1" t="n">
-        <v>0.80554</v>
-      </c>
-      <c r="V18" s="1" t="n">
-        <v>0.80554</v>
-      </c>
-      <c r="W18" s="1" t="n">
-        <v>0.80554</v>
-      </c>
-      <c r="X18" s="1" t="n">
-        <v>0.79066</v>
-      </c>
-      <c r="Y18" s="1" t="n">
-        <v>0.646260003</v>
-      </c>
-      <c r="Z18" s="1" t="n">
-        <v>0.596</v>
-      </c>
-      <c r="AA18" s="1" t="n">
-        <v>0.5835126856</v>
-      </c>
-      <c r="AB18" s="1" t="n">
-        <v>0.7164726998</v>
-      </c>
-      <c r="AC18" s="1" t="n">
-        <v>0.6716458456</v>
-      </c>
-      <c r="AD18" s="1" t="n">
-        <v>0.665115796</v>
-      </c>
-      <c r="AE18" s="1" t="n">
-        <v>0.4906097</v>
-      </c>
-      <c r="AF18" s="1" t="n">
-        <v>0.4807676</v>
-      </c>
-      <c r="AG18" s="1" t="n">
-        <v>0.4941387</v>
-      </c>
-      <c r="AH18" s="1" t="n">
-        <v>0.4941387</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <v>0.11878</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <v>0.11878</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>0.11956</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>0.12035</v>
-      </c>
-      <c r="J19" s="1" t="n">
-        <v>0.12218</v>
-      </c>
-      <c r="K19" s="1" t="n">
-        <v>0.124013</v>
-      </c>
-      <c r="L19" s="1" t="n">
-        <v>0.125357</v>
-      </c>
-      <c r="M19" s="1" t="n">
-        <v>0.66961</v>
-      </c>
-      <c r="N19" s="1" t="n">
-        <v>0.66961</v>
-      </c>
-      <c r="O19" s="1" t="n">
-        <v>0.69627</v>
-      </c>
-      <c r="P19" s="1" t="n">
-        <v>0.69627</v>
-      </c>
-      <c r="Q19" s="1" t="n">
-        <v>0.00054</v>
-      </c>
-      <c r="R19" s="1" t="n">
-        <v>0.00054</v>
-      </c>
-      <c r="S19" s="1" t="n">
-        <v>0.00054</v>
-      </c>
-      <c r="T19" s="1" t="n">
-        <v>0.00054</v>
-      </c>
-      <c r="U19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="M20" s="1" t="n">
-        <v>0.4893</v>
-      </c>
-      <c r="N20" s="1" t="n">
-        <v>0.4893</v>
-      </c>
-      <c r="O20" s="1" t="n">
-        <v>0.712000008</v>
-      </c>
-      <c r="P20" s="1" t="n">
-        <v>0.712000008</v>
-      </c>
-      <c r="Q20" s="1" t="n">
-        <v>0.0065099998</v>
-      </c>
-      <c r="R20" s="1" t="n">
-        <v>0.0065099998</v>
-      </c>
-      <c r="S20" s="1" t="n">
-        <v>0.0065099998</v>
-      </c>
-      <c r="T20" s="1" t="n">
-        <v>0.0065099998</v>
-      </c>
-      <c r="U20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1047995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1047996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1047997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1047998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1047999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048013" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048014" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048015" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048016" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048017" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048018" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048019" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048020" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048021" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048022" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048023" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048024" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048025" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048026" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048027" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048028" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048029" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048030" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048031" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048032" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048033" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048034" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048035" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048036" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048037" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048038" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048039" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048040" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048041" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048042" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048043" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048044" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048045" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048046" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048047" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048048" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048049" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048050" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048051" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048052" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048053" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048054" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048055" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048056" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048057" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048058" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048059" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048060" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048061" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048062" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048063" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048064" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048065" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048066" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048067" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048068" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048069" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048070" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048071" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048072" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048073" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048074" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048076" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048077" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048078" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048079" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048080" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048081" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048082" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048083" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048084" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048085" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048086" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048087" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048088" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048089" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048090" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048091" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048092" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048093" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048094" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048095" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048096" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048097" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048098" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048099" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:AH20"/>
+  <autoFilter ref="A2:AH8"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>